<commit_message>
Up to page 140.  Inserting page numbers and converting Bible refs.
</commit_message>
<xml_diff>
--- a/dev/text/ministry/Page Number Finder.xlsx
+++ b/dev/text/ministry/Page Number Finder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\ministry\dev\text\ministry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0754E4D1-C1A3-4CA1-A41A-16278E064EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF7B626-3368-4AA7-B4D7-5CBD3AAAFF79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{78E5F7DC-C11E-49DB-B1EE-13CE08E681FE}"/>
+    <workbookView xWindow="3588" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{78E5F7DC-C11E-49DB-B1EE-13CE08E681FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2356,7 +2356,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D756F75-117D-4589-A963-F6E7419A4C4B}">
   <dimension ref="A1:B328"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="A140" sqref="A140"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3822,7 +3824,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A184" s="2" t="s">
         <v>431</v>
       </c>

</xml_diff>